<commit_message>
Clean up Part 3 and save CMS rates
</commit_message>
<xml_diff>
--- a/qf605-fixed-income/data/sabr_calibrated.xlsx
+++ b/qf605-fixed-income/data/sabr_calibrated.xlsx
@@ -469,19 +469,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1391177694231066</v>
+        <v>0.1391035778845959</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1846311437361156</v>
+        <v>0.1846425592601795</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1968245453932313</v>
+        <v>0.1967712904214697</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1781495538911682</v>
+        <v>0.1779273404887576</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1727589651188632</v>
+        <v>0.172890201220095</v>
       </c>
     </row>
     <row r="3">
@@ -491,19 +491,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1666405030017211</v>
+        <v>0.1664545218569979</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1986920640478133</v>
+        <v>0.1983862754120166</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1999451847614024</v>
+        <v>0.1999508905666859</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1883856878566519</v>
+        <v>0.1880623432715516</v>
       </c>
       <c r="F3" t="n">
-        <v>0.17063106637228</v>
+        <v>0.171354499666421</v>
       </c>
     </row>
     <row r="4">
@@ -513,19 +513,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1766681763817387</v>
+        <v>0.1783943026753877</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1926930765646341</v>
+        <v>0.1932472883083041</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1965753688622109</v>
+        <v>0.1968208170551125</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1926050870219206</v>
+        <v>0.1929909483890378</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1773786194049607</v>
+        <v>0.1789472682163097</v>
       </c>
     </row>
   </sheetData>
@@ -581,19 +581,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.6329876681687155</v>
+        <v>-0.6330062548889566</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.525337597569106</v>
+        <v>-0.5250855973782115</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.4831297395439832</v>
+        <v>-0.4826171172249953</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.4165000751703339</v>
+        <v>-0.4136425277006885</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.3080300238788374</v>
+        <v>-0.3097880589022577</v>
       </c>
     </row>
     <row r="3">
@@ -603,19 +603,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.5843784817874683</v>
+        <v>-0.5851338342383721</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.5451623032059372</v>
+        <v>-0.5438848697963986</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.5192037559179212</v>
+        <v>-0.5179597068906967</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.498743074072418</v>
+        <v>-0.4957420723203845</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.3901202644965844</v>
+        <v>-0.3971619656711662</v>
       </c>
     </row>
     <row r="4">
@@ -625,19 +625,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.5525023448268775</v>
+        <v>-0.5488092695261677</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.5453249721517903</v>
+        <v>-0.540522024976866</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.5315120167547526</v>
+        <v>-0.5276708274378461</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.5404873546671907</v>
+        <v>-0.540684142814833</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.5084018917440672</v>
+        <v>-0.5127356878951527</v>
       </c>
     </row>
   </sheetData>
@@ -693,19 +693,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.049198633956934</v>
+        <v>2.048783209110644</v>
       </c>
       <c r="C2" t="n">
-        <v>1.679633689423351</v>
+        <v>1.677390418935748</v>
       </c>
       <c r="D2" t="n">
-        <v>1.441003835359067</v>
+        <v>1.438553967961835</v>
       </c>
       <c r="E2" t="n">
-        <v>1.066331560365873</v>
+        <v>1.066043910350141</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7699940557453125</v>
+        <v>0.7604156618523644</v>
       </c>
     </row>
     <row r="3">
@@ -715,19 +715,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.332680149730216</v>
+        <v>1.339865494949765</v>
       </c>
       <c r="C3" t="n">
-        <v>1.064564699296813</v>
+        <v>1.062308192887452</v>
       </c>
       <c r="D3" t="n">
-        <v>0.953271385366513</v>
+        <v>0.9467116104193644</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6880500324821187</v>
+        <v>0.6835419435497165</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5533080301251064</v>
+        <v>0.5433373638486673</v>
       </c>
     </row>
     <row r="4">
@@ -737,19 +737,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.040785710879257</v>
+        <v>1.010697794727172</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9502018101951232</v>
+        <v>0.9245785503057192</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8796305578792002</v>
+        <v>0.8608700206026637</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7296450726108302</v>
+        <v>0.7236644034101184</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6199948348583607</v>
+        <v>0.6015151318353243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ann qf605 project convert to .py
</commit_message>
<xml_diff>
--- a/qf605-fixed-income/data/sabr_calibrated.xlsx
+++ b/qf605-fixed-income/data/sabr_calibrated.xlsx
@@ -469,7 +469,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1391035778845959</v>
+        <v>0.1390971420698965</v>
       </c>
       <c r="C2" t="n">
         <v>0.1846425592601795</v>
@@ -478,10 +478,10 @@
         <v>0.1967712904214697</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1779273404887576</v>
+        <v>0.1779276634019181</v>
       </c>
       <c r="F2" t="n">
-        <v>0.172890201220095</v>
+        <v>0.1728902981320911</v>
       </c>
     </row>
     <row r="3">
@@ -491,19 +491,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1664545218569979</v>
+        <v>0.1664651213615663</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1983862754120166</v>
+        <v>0.1983862847089853</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1999508905666859</v>
+        <v>0.1999398997549089</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1880623432715516</v>
+        <v>0.1880623463175923</v>
       </c>
       <c r="F3" t="n">
-        <v>0.171354499666421</v>
+        <v>0.1713547357308199</v>
       </c>
     </row>
     <row r="4">
@@ -513,19 +513,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1783943026753877</v>
+        <v>0.1783943025676695</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1932472883083041</v>
+        <v>0.1932472945943859</v>
       </c>
       <c r="D4" t="n">
         <v>0.1968208170551125</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1929909483890378</v>
+        <v>0.1929910278893894</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1789472682163097</v>
+        <v>0.179340894856134</v>
       </c>
     </row>
   </sheetData>
@@ -581,7 +581,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.6330062548889566</v>
+        <v>-0.6330083290141738</v>
       </c>
       <c r="C2" t="n">
         <v>-0.5250855973782115</v>
@@ -590,10 +590,10 @@
         <v>-0.4826171172249953</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.4136425277006885</v>
+        <v>-0.4136398249487697</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.3097880589022577</v>
+        <v>-0.309871243281606</v>
       </c>
     </row>
     <row r="3">
@@ -603,19 +603,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.5851338342383721</v>
+        <v>-0.5851633008555246</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.5438848697963986</v>
+        <v>-0.5438848952462392</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.5179597068906967</v>
+        <v>-0.5179704478048697</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.4957420723203845</v>
+        <v>-0.4957420879509322</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.3971619656711662</v>
+        <v>-0.3971620072285023</v>
       </c>
     </row>
     <row r="4">
@@ -625,19 +625,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.5488092695261677</v>
+        <v>-0.5488092691787519</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.540522024976866</v>
+        <v>-0.540522029067068</v>
       </c>
       <c r="D4" t="n">
         <v>-0.5276708274378461</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.540684142814833</v>
+        <v>-0.5406862335741107</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.5127356878951527</v>
+        <v>-0.5135209302351936</v>
       </c>
     </row>
   </sheetData>
@@ -693,7 +693,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.048783209110644</v>
+        <v>2.048776744257994</v>
       </c>
       <c r="C2" t="n">
         <v>1.677390418935748</v>
@@ -702,10 +702,10 @@
         <v>1.438553967961835</v>
       </c>
       <c r="E2" t="n">
-        <v>1.066043910350141</v>
+        <v>1.066048324656234</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7604156618523644</v>
+        <v>0.7603655000109073</v>
       </c>
     </row>
     <row r="3">
@@ -715,19 +715,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.339865494949765</v>
+        <v>1.33991682782383</v>
       </c>
       <c r="C3" t="n">
-        <v>1.062308192887452</v>
+        <v>1.062308186442275</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9467116104193644</v>
+        <v>0.9468147157189183</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6835419435497165</v>
+        <v>0.6835419337291175</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5433373638486673</v>
+        <v>0.5433371927042306</v>
       </c>
     </row>
     <row r="4">
@@ -737,19 +737,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.010697794727172</v>
+        <v>1.010697794389251</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9245785503057192</v>
+        <v>0.9245785345258318</v>
       </c>
       <c r="D4" t="n">
         <v>0.8608700206026637</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7236644034101184</v>
+        <v>0.7236637617522718</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6015151318353243</v>
+        <v>0.5991036936418281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>